<commit_message>
Adding Macro Schedule Detail import code and all SQL Scripts for table creation.
</commit_message>
<xml_diff>
--- a/src/SFA/wwwroot/resources/macroSchedules/macroSchedule.xlsx
+++ b/src/SFA/wwwroot/resources/macroSchedules/macroSchedule.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SEANR\OneDrive\Documents\GitHub\gmdeputation\src\SFA\wwwroot\resources\macroSchedules\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEF703F-656E-4710-8F1B-DB44D64650BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="8520"/>
+    <workbookView xWindow="-26205" yWindow="3030" windowWidth="22785" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,55 +22,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Schedule Description</t>
-  </si>
-  <si>
-    <t>Entry Date</t>
-  </si>
-  <si>
-    <t>Missionary ID</t>
-  </si>
-  <si>
-    <t>Start Date</t>
-  </si>
-  <si>
-    <t>End Date</t>
   </si>
   <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>ok</t>
+    <t>UserId</t>
   </si>
   <si>
-    <t>District No</t>
+    <t>Start Date MM/dd/yyyy</t>
   </si>
   <si>
-    <t>Test Schedule</t>
-  </si>
-  <si>
-    <t>M000040</t>
-  </si>
-  <si>
-    <t>03/20/2020</t>
-  </si>
-  <si>
-    <t>03/25/2020</t>
-  </si>
-  <si>
-    <t>03/27/2020</t>
-  </si>
-  <si>
-    <t>Note : Date should be 'MM/dd/yyyy' format and string format in excel value</t>
+    <t>End Date MM/dd/yyyy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,20 +80,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -161,7 +144,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -193,9 +176,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -227,6 +228,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -402,108 +421,69 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:G5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="20.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A5:G5"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated import for Macro Schedule/Deatails to include district ID
</commit_message>
<xml_diff>
--- a/src/SFA/wwwroot/resources/macroSchedules/macroSchedule.xlsx
+++ b/src/SFA/wwwroot/resources/macroSchedules/macroSchedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SEANR\OneDrive\Documents\GitHub\gmdeputation\src\SFA\wwwroot\resources\macroSchedules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEF703F-656E-4710-8F1B-DB44D64650BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C32E65B-EAF8-4655-891F-88D15D2F1F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26205" yWindow="3030" windowWidth="22785" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26160" yWindow="2970" windowWidth="22785" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Schedule Description</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>End Date MM/dd/yyyy</t>
+  </si>
+  <si>
+    <t>District ID</t>
   </si>
 </sst>
 </file>
@@ -425,7 +428,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +437,8 @@
     <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -452,6 +456,9 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>